<commit_message>
modificato directory nel file_dogana
</commit_message>
<xml_diff>
--- a/Off_White/Negozi.xlsx
+++ b/Off_White/Negozi.xlsx
@@ -1,14 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" rupBuild="4506" lastEdited="4" lowestEdited="4"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miche\Desktop\py\GitHub\Python\Off_White\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA77561F-9B57-4FC0-9026-4679BD0B7947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="14370"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="flId1"/>
+    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -336,7 +343,7 @@
     <t>5JPV4QP0H</t>
   </si>
   <si>
-    <t xml:space="preserve">VOLCANITE SUNGLASSES BLACK DARK GREY   BLACK DARK GREY</t>
+    <t>VOLCANITE SUNGLASSES BLACK DARK GREY   BLACK DARK GREY</t>
   </si>
   <si>
     <t>100% injected</t>
@@ -417,169 +424,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Cambria"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -592,207 +441,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.799981688894314" theme="4"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.799981688894314" theme="5"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.799981688894314" theme="6"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.599993896298105" theme="7"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.799981688894314" theme="8"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.799981688894314" theme="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.599993896298105" theme="8"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.399975585192419" theme="5"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.399975585192419" theme="6"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.599993896298105" theme="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.399975585192419" theme="4"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.399975585192419" theme="7"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.399975585192419" theme="8"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.399975585192419" theme="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.599993896298105" theme="4"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.599993896298105" theme="5"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.599993896298105" theme="6"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor tint="0.799981688894314" theme="7"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -800,268 +457,35 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color tint="0.499984740745262" theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color tint="0.399975585192419" theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="61">
-    <xf fontId="0" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="1" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="1" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="2" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="2" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="2" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="3" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="4" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="32" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="6" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="7" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="28" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="29" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="30" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="5" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="8" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="11" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="12" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="9" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="10" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="13" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="14" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="15" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="16" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="17" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="18" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="31" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="33" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="19" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="10" numFmtId="0" fillId="25" borderId="0"/>
-    <xf applyNumberFormat="0" applyAlignment="0" applyProtection="0" fontId="14" numFmtId="0" fillId="20" borderId="1"/>
-    <xf applyNumberFormat="0" applyAlignment="0" applyProtection="0" fontId="16" numFmtId="0" fillId="21" borderId="2"/>
-    <xf applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="43" fillId="0" borderId="0"/>
-    <xf applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="41" fillId="0" borderId="0"/>
-    <xf applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="44" fillId="0" borderId="0"/>
-    <xf applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="42" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="18" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="9" numFmtId="0" fillId="24" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" fontId="6" numFmtId="0" fillId="0" borderId="3"/>
-    <xf applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" fontId="7" numFmtId="0" fillId="0" borderId="4"/>
-    <xf applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" fontId="8" numFmtId="0" fillId="0" borderId="5"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="8" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyAlignment="0" applyProtection="0" fontId="12" numFmtId="0" fillId="26" borderId="1"/>
-    <xf applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" fontId="15" numFmtId="0" fillId="0" borderId="6"/>
-    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="11" numFmtId="0" fillId="22" borderId="0"/>
-    <xf applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="23" borderId="7"/>
-    <xf applyNumberFormat="0" applyAlignment="0" applyProtection="0" fontId="13" numFmtId="0" fillId="20" borderId="8"/>
-    <xf applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="9" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="5" numFmtId="0" fillId="0" borderId="0"/>
-    <xf applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" fontId="19" numFmtId="0" fillId="0" borderId="9"/>
-    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="17" numFmtId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf fontId="0" numFmtId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf applyFont="1" fontId="21" numFmtId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf applyNumberFormat="1" applyFont="1" fontId="21" numFmtId="14" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="61">
-    <cellStyle name="20% - Accent1" xfId="15" builtinId="30"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="20% - Accent3" xfId="17" builtinId="38"/>
-    <cellStyle name="20% - Accent4" xfId="18" builtinId="42"/>
-    <cellStyle name="20% - Accent5" xfId="19" builtinId="46"/>
-    <cellStyle name="20% - Accent6" xfId="20" builtinId="50"/>
-    <cellStyle name="40% - Accent1" xfId="21" builtinId="31"/>
-    <cellStyle name="40% - Accent2" xfId="22" builtinId="35"/>
-    <cellStyle name="40% - Accent3" xfId="23" builtinId="39"/>
-    <cellStyle name="40% - Accent4" xfId="24" builtinId="43"/>
-    <cellStyle name="40% - Accent5" xfId="25" builtinId="47"/>
-    <cellStyle name="40% - Accent6" xfId="26" builtinId="51"/>
-    <cellStyle name="60% - Accent1" xfId="27" builtinId="32"/>
-    <cellStyle name="60% - Accent2" xfId="28" builtinId="36"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40"/>
-    <cellStyle name="60% - Accent4" xfId="30" builtinId="44"/>
-    <cellStyle name="60% - Accent5" xfId="31" builtinId="48"/>
-    <cellStyle name="60% - Accent6" xfId="32" builtinId="52"/>
-    <cellStyle name="Accent1" xfId="33" builtinId="29"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="Accent3" xfId="35" builtinId="37"/>
-    <cellStyle name="Accent4" xfId="36" builtinId="41"/>
-    <cellStyle name="Accent5" xfId="37" builtinId="45"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49"/>
-    <cellStyle name="Bad" xfId="39" builtinId="27"/>
-    <cellStyle name="Calculation" xfId="40" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="41" builtinId="23"/>
-    <cellStyle name="ColLevel_1" xfId="2" builtinId="2" iLevel="0"/>
-    <cellStyle name="ColLevel_2" xfId="4" builtinId="2" iLevel="1"/>
-    <cellStyle name="ColLevel_3" xfId="6" builtinId="2" iLevel="2"/>
-    <cellStyle name="ColLevel_4" xfId="8" builtinId="2" iLevel="3"/>
-    <cellStyle name="ColLevel_5" xfId="10" builtinId="2" iLevel="4"/>
-    <cellStyle name="ColLevel_6" xfId="12" builtinId="2" iLevel="5"/>
-    <cellStyle name="ColLevel_7" xfId="14" builtinId="2" iLevel="6"/>
-    <cellStyle name="Comma" xfId="42" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="43" builtinId="6"/>
-    <cellStyle name="Currency" xfId="44" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="45" builtinId="7"/>
-    <cellStyle name="Explanatory Text" xfId="46" builtinId="53"/>
-    <cellStyle name="Good" xfId="47" builtinId="26"/>
-    <cellStyle name="Heading 1" xfId="48" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="49" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="50" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="51" builtinId="19"/>
-    <cellStyle name="Input" xfId="52" builtinId="20"/>
-    <cellStyle name="Linked Cell" xfId="53" builtinId="24"/>
-    <cellStyle name="Neutral" xfId="54" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="55" builtinId="10"/>
-    <cellStyle name="Output" xfId="56" builtinId="21"/>
-    <cellStyle name="Percent" xfId="57" builtinId="5"/>
-    <cellStyle name="RowLevel_1" xfId="1" builtinId="1" iLevel="0"/>
-    <cellStyle name="RowLevel_2" xfId="3" builtinId="1" iLevel="1"/>
-    <cellStyle name="RowLevel_3" xfId="5" builtinId="1" iLevel="2"/>
-    <cellStyle name="RowLevel_4" xfId="7" builtinId="1" iLevel="3"/>
-    <cellStyle name="RowLevel_5" xfId="9" builtinId="1" iLevel="4"/>
-    <cellStyle name="RowLevel_6" xfId="11" builtinId="1" iLevel="5"/>
-    <cellStyle name="RowLevel_7" xfId="13" builtinId="1" iLevel="6"/>
-    <cellStyle name="Title" xfId="58" builtinId="15"/>
-    <cellStyle name="Total" xfId="59" builtinId="25"/>
-    <cellStyle name="Warning Text" xfId="60" builtinId="11"/>
+  <cellStyles count="1">
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1099,9 +523,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1134,26 +558,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1186,26 +593,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1311,12 +701,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1378,49 +768,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.73046875" customWidth="1"/>
-    <col min="2" max="2" width="16.4765625" customWidth="1"/>
-    <col min="3" max="3" width="10.11328125" customWidth="1"/>
-    <col min="4" max="4" width="14.8984375" customWidth="1"/>
-    <col min="5" max="5" width="21.4609375" customWidth="1"/>
-    <col min="6" max="6" width="9.28125" customWidth="1"/>
-    <col min="7" max="7" width="57.32421875" customWidth="1"/>
-    <col min="8" max="8" width="7.3515625" customWidth="1"/>
-    <col min="9" max="9" width="5.15234375" customWidth="1"/>
-    <col min="10" max="10" width="7.46875" customWidth="1"/>
-    <col min="11" max="11" width="8.96484375" customWidth="1"/>
-    <col min="12" max="12" width="2.9140625" customWidth="1"/>
-    <col min="13" max="13" width="6.83984375" customWidth="1"/>
-    <col min="14" max="14" width="8.92578125" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="57.28515625" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="12" max="12" width="2.85546875" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" customWidth="1"/>
     <col min="15" max="15" width="21.42578125" customWidth="1"/>
-    <col min="16" max="16" width="11.8515625" customWidth="1"/>
-    <col min="17" max="17" width="15.00390625" customWidth="1"/>
-    <col min="18" max="18" width="10.82421875" customWidth="1"/>
-    <col min="19" max="19" width="14.01953125" customWidth="1"/>
-    <col min="20" max="20" width="16.8984375" customWidth="1"/>
-    <col min="21" max="21" width="6.77734375" customWidth="1"/>
-    <col min="22" max="22" width="5.8359375" customWidth="1"/>
-    <col min="23" max="23" width="6.8671875" customWidth="1"/>
-    <col min="24" max="24" width="4.48046875" customWidth="1"/>
-    <col min="25" max="25" width="11.875" customWidth="1"/>
-    <col min="26" max="26" width="14.46484375" customWidth="1"/>
-    <col min="27" max="27" width="18.33203125" customWidth="1"/>
-    <col min="28" max="28" width="16.2890625" customWidth="1"/>
-    <col min="29" max="29" width="11.80859375" customWidth="1"/>
-    <col min="30" max="30" width="13.60546875" customWidth="1"/>
-    <col min="31" max="31" width="11.65234375" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" customWidth="1"/>
+    <col min="17" max="17" width="15" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" customWidth="1"/>
+    <col min="19" max="19" width="14" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" customWidth="1"/>
+    <col min="22" max="22" width="5.85546875" customWidth="1"/>
+    <col min="23" max="23" width="6.85546875" customWidth="1"/>
+    <col min="24" max="24" width="4.42578125" customWidth="1"/>
+    <col min="25" max="25" width="11.85546875" customWidth="1"/>
+    <col min="26" max="26" width="14.42578125" customWidth="1"/>
+    <col min="27" max="27" width="18.28515625" customWidth="1"/>
+    <col min="28" max="28" width="16.28515625" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" customWidth="1"/>
+    <col min="30" max="30" width="13.5703125" customWidth="1"/>
+    <col min="31" max="31" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1515,7 +906,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -1594,7 +985,7 @@
       </c>
       <c r="AE2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1673,7 +1064,7 @@
       </c>
       <c r="AE3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1752,7 +1143,7 @@
       </c>
       <c r="AE4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -1831,7 +1222,7 @@
       </c>
       <c r="AE5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -1910,7 +1301,7 @@
       </c>
       <c r="AE6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1976,7 +1367,7 @@
         <v>0</v>
       </c>
       <c r="AA7" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AB7" s="1">
         <v>0</v>
@@ -1989,7 +1380,7 @@
       </c>
       <c r="AE7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -2068,7 +1459,7 @@
       </c>
       <c r="AE8" s="1"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -2147,7 +1538,7 @@
       </c>
       <c r="AE9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -2226,7 +1617,7 @@
       </c>
       <c r="AE10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -2305,7 +1696,7 @@
       </c>
       <c r="AE11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -2384,7 +1775,7 @@
       </c>
       <c r="AE12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -2463,7 +1854,7 @@
       </c>
       <c r="AE13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -2529,7 +1920,7 @@
         <v>0</v>
       </c>
       <c r="AA14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB14" s="1">
         <v>0</v>
@@ -2542,7 +1933,7 @@
       </c>
       <c r="AE14" s="1"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -2621,7 +2012,7 @@
       </c>
       <c r="AE15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -2700,7 +2091,7 @@
       </c>
       <c r="AE16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -2779,7 +2170,7 @@
       </c>
       <c r="AE17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -2858,7 +2249,7 @@
       </c>
       <c r="AE18" s="1"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -2937,7 +2328,7 @@
       </c>
       <c r="AE19" s="1"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -3016,7 +2407,7 @@
       </c>
       <c r="AE20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -3084,7 +2475,7 @@
         <v>0</v>
       </c>
       <c r="AA21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB21" s="1">
         <v>0</v>
@@ -3097,7 +2488,7 @@
       </c>
       <c r="AE21" s="1"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -3178,7 +2569,7 @@
       </c>
       <c r="AE22" s="1"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
@@ -3259,7 +2650,7 @@
       </c>
       <c r="AE23" s="1"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>123</v>
       </c>
@@ -3338,7 +2729,7 @@
       </c>
       <c r="AE24" s="1"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>123</v>
       </c>
@@ -3417,7 +2808,7 @@
       </c>
       <c r="AE25" s="1"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>123</v>
       </c>
@@ -3496,7 +2887,7 @@
       </c>
       <c r="AE26" s="1"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>123</v>
       </c>
@@ -3562,7 +2953,7 @@
         <v>0</v>
       </c>
       <c r="AA27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB27" s="1">
         <v>0</v>
@@ -3575,7 +2966,7 @@
       </c>
       <c r="AE27" s="1"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>123</v>
       </c>
@@ -3641,7 +3032,7 @@
         <v>0</v>
       </c>
       <c r="AA28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB28" s="1">
         <v>0</v>
@@ -3654,7 +3045,7 @@
       </c>
       <c r="AE28" s="1"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>123</v>
       </c>
@@ -3720,7 +3111,7 @@
         <v>0</v>
       </c>
       <c r="AA29" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB29" s="1">
         <v>0</v>
@@ -3733,7 +3124,7 @@
       </c>
       <c r="AE29" s="1"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>123</v>
       </c>
@@ -3812,7 +3203,7 @@
       </c>
       <c r="AE30" s="1"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>123</v>
       </c>
@@ -3891,7 +3282,7 @@
       </c>
       <c r="AE31" s="1"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>123</v>
       </c>
@@ -3972,6 +3363,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup usePrinterDefaults="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
aggiunto readme a teerayuth
</commit_message>
<xml_diff>
--- a/Off_White/Negozi.xlsx
+++ b/Off_White/Negozi.xlsx
@@ -1,21 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" rupBuild="4506" lastEdited="4" lowestEdited="4"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miche\Desktop\py\GitHub\Python\Off_White\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA77561F-9B57-4FC0-9026-4679BD0B7947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="14370"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio1" sheetId="1" r:id="flId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -343,7 +336,7 @@
     <t>5JPV4QP0H</t>
   </si>
   <si>
-    <t>VOLCANITE SUNGLASSES BLACK DARK GREY   BLACK DARK GREY</t>
+    <t xml:space="preserve">VOLCANITE SUNGLASSES BLACK DARK GREY   BLACK DARK GREY</t>
   </si>
   <si>
     <t>100% injected</t>
@@ -424,11 +417,169 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -441,15 +592,207 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.799981688894314" theme="4"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.799981688894314" theme="5"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.799981688894314" theme="6"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.599993896298105" theme="7"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.799981688894314" theme="8"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.799981688894314" theme="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.599993896298105" theme="8"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.399975585192419" theme="5"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.399975585192419" theme="6"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.599993896298105" theme="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.399975585192419" theme="4"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.399975585192419" theme="7"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.399975585192419" theme="8"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.399975585192419" theme="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.599993896298105" theme="4"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.599993896298105" theme="5"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.599993896298105" theme="6"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor tint="0.799981688894314" theme="7"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -457,35 +800,268 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color tint="0.499984740745262" theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color tint="0.399975585192419" theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="61">
+    <xf fontId="0" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="1" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="1" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="2" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="2" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="0" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="2" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="3" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="4" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="32" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="6" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="7" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="28" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="29" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="30" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="5" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="8" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="11" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="12" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="9" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="10" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="13" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="14" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="15" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="16" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="17" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="18" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="31" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="33" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="20" numFmtId="0" fillId="19" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="10" numFmtId="0" fillId="25" borderId="0"/>
+    <xf applyNumberFormat="0" applyAlignment="0" applyProtection="0" fontId="14" numFmtId="0" fillId="20" borderId="1"/>
+    <xf applyNumberFormat="0" applyAlignment="0" applyProtection="0" fontId="16" numFmtId="0" fillId="21" borderId="2"/>
+    <xf applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="43" fillId="0" borderId="0"/>
+    <xf applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="41" fillId="0" borderId="0"/>
+    <xf applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="44" fillId="0" borderId="0"/>
+    <xf applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="42" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="18" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="9" numFmtId="0" fillId="24" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" fontId="6" numFmtId="0" fillId="0" borderId="3"/>
+    <xf applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" fontId="7" numFmtId="0" fillId="0" borderId="4"/>
+    <xf applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" fontId="8" numFmtId="0" fillId="0" borderId="5"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="8" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyAlignment="0" applyProtection="0" fontId="12" numFmtId="0" fillId="26" borderId="1"/>
+    <xf applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" fontId="15" numFmtId="0" fillId="0" borderId="6"/>
+    <xf applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="11" numFmtId="0" fillId="22" borderId="0"/>
+    <xf applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="0" fillId="23" borderId="7"/>
+    <xf applyNumberFormat="0" applyAlignment="0" applyProtection="0" fontId="13" numFmtId="0" fillId="20" borderId="8"/>
+    <xf applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="4" numFmtId="9" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="5" numFmtId="0" fillId="0" borderId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" fontId="19" numFmtId="0" fillId="0" borderId="9"/>
+    <xf applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" fontId="17" numFmtId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf fontId="0" numFmtId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf applyFont="1" fontId="21" numFmtId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf applyNumberFormat="1" applyFont="1" fontId="21" numFmtId="14" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+  <cellStyles count="61">
+    <cellStyle name="20% - Accent1" xfId="15" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="20% - Accent3" xfId="17" builtinId="38"/>
+    <cellStyle name="20% - Accent4" xfId="18" builtinId="42"/>
+    <cellStyle name="20% - Accent5" xfId="19" builtinId="46"/>
+    <cellStyle name="20% - Accent6" xfId="20" builtinId="50"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31"/>
+    <cellStyle name="40% - Accent2" xfId="22" builtinId="35"/>
+    <cellStyle name="40% - Accent3" xfId="23" builtinId="39"/>
+    <cellStyle name="40% - Accent4" xfId="24" builtinId="43"/>
+    <cellStyle name="40% - Accent5" xfId="25" builtinId="47"/>
+    <cellStyle name="40% - Accent6" xfId="26" builtinId="51"/>
+    <cellStyle name="60% - Accent1" xfId="27" builtinId="32"/>
+    <cellStyle name="60% - Accent2" xfId="28" builtinId="36"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40"/>
+    <cellStyle name="60% - Accent4" xfId="30" builtinId="44"/>
+    <cellStyle name="60% - Accent5" xfId="31" builtinId="48"/>
+    <cellStyle name="60% - Accent6" xfId="32" builtinId="52"/>
+    <cellStyle name="Accent1" xfId="33" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="Accent3" xfId="35" builtinId="37"/>
+    <cellStyle name="Accent4" xfId="36" builtinId="41"/>
+    <cellStyle name="Accent5" xfId="37" builtinId="45"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49"/>
+    <cellStyle name="Bad" xfId="39" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="40" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="41" builtinId="23"/>
+    <cellStyle name="ColLevel_1" xfId="2" builtinId="2" iLevel="0"/>
+    <cellStyle name="ColLevel_2" xfId="4" builtinId="2" iLevel="1"/>
+    <cellStyle name="ColLevel_3" xfId="6" builtinId="2" iLevel="2"/>
+    <cellStyle name="ColLevel_4" xfId="8" builtinId="2" iLevel="3"/>
+    <cellStyle name="ColLevel_5" xfId="10" builtinId="2" iLevel="4"/>
+    <cellStyle name="ColLevel_6" xfId="12" builtinId="2" iLevel="5"/>
+    <cellStyle name="ColLevel_7" xfId="14" builtinId="2" iLevel="6"/>
+    <cellStyle name="Comma" xfId="42" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="43" builtinId="6"/>
+    <cellStyle name="Currency" xfId="44" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="45" builtinId="7"/>
+    <cellStyle name="Explanatory Text" xfId="46" builtinId="53"/>
+    <cellStyle name="Good" xfId="47" builtinId="26"/>
+    <cellStyle name="Heading 1" xfId="48" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="49" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="50" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="51" builtinId="19"/>
+    <cellStyle name="Input" xfId="52" builtinId="20"/>
+    <cellStyle name="Linked Cell" xfId="53" builtinId="24"/>
+    <cellStyle name="Neutral" xfId="54" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="55" builtinId="10"/>
+    <cellStyle name="Output" xfId="56" builtinId="21"/>
+    <cellStyle name="Percent" xfId="57" builtinId="5"/>
+    <cellStyle name="RowLevel_1" xfId="1" builtinId="1" iLevel="0"/>
+    <cellStyle name="RowLevel_2" xfId="3" builtinId="1" iLevel="1"/>
+    <cellStyle name="RowLevel_3" xfId="5" builtinId="1" iLevel="2"/>
+    <cellStyle name="RowLevel_4" xfId="7" builtinId="1" iLevel="3"/>
+    <cellStyle name="RowLevel_5" xfId="9" builtinId="1" iLevel="4"/>
+    <cellStyle name="RowLevel_6" xfId="11" builtinId="1" iLevel="5"/>
+    <cellStyle name="RowLevel_7" xfId="13" builtinId="1" iLevel="6"/>
+    <cellStyle name="Title" xfId="58" builtinId="15"/>
+    <cellStyle name="Total" xfId="59" builtinId="25"/>
+    <cellStyle name="Warning Text" xfId="60" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -523,9 +1099,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -558,9 +1134,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,9 +1186,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -701,12 +1311,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -768,50 +1378,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" topLeftCell="A1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" customWidth="1"/>
-    <col min="7" max="7" width="57.28515625" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" customWidth="1"/>
-    <col min="9" max="9" width="5.140625" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="12" max="12" width="2.85546875" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.73046875" customWidth="1"/>
+    <col min="2" max="2" width="16.4765625" customWidth="1"/>
+    <col min="3" max="3" width="10.11328125" customWidth="1"/>
+    <col min="4" max="4" width="14.8984375" customWidth="1"/>
+    <col min="5" max="5" width="21.4609375" customWidth="1"/>
+    <col min="6" max="6" width="9.28125" customWidth="1"/>
+    <col min="7" max="7" width="57.32421875" customWidth="1"/>
+    <col min="8" max="8" width="7.3515625" customWidth="1"/>
+    <col min="9" max="9" width="5.15234375" customWidth="1"/>
+    <col min="10" max="10" width="7.46875" customWidth="1"/>
+    <col min="11" max="11" width="8.96484375" customWidth="1"/>
+    <col min="12" max="12" width="2.9140625" customWidth="1"/>
+    <col min="13" max="13" width="6.83984375" customWidth="1"/>
+    <col min="14" max="14" width="8.92578125" customWidth="1"/>
     <col min="15" max="15" width="21.42578125" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" customWidth="1"/>
-    <col min="17" max="17" width="15" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" customWidth="1"/>
-    <col min="19" max="19" width="14" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" customWidth="1"/>
-    <col min="21" max="21" width="6.7109375" customWidth="1"/>
-    <col min="22" max="22" width="5.85546875" customWidth="1"/>
-    <col min="23" max="23" width="6.85546875" customWidth="1"/>
-    <col min="24" max="24" width="4.42578125" customWidth="1"/>
-    <col min="25" max="25" width="11.85546875" customWidth="1"/>
-    <col min="26" max="26" width="14.42578125" customWidth="1"/>
-    <col min="27" max="27" width="18.28515625" customWidth="1"/>
-    <col min="28" max="28" width="16.28515625" customWidth="1"/>
-    <col min="29" max="29" width="11.85546875" customWidth="1"/>
-    <col min="30" max="30" width="13.5703125" customWidth="1"/>
-    <col min="31" max="31" width="11.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.8515625" customWidth="1"/>
+    <col min="17" max="17" width="15.00390625" customWidth="1"/>
+    <col min="18" max="18" width="10.82421875" customWidth="1"/>
+    <col min="19" max="19" width="14.01953125" customWidth="1"/>
+    <col min="20" max="20" width="16.8984375" customWidth="1"/>
+    <col min="21" max="21" width="6.77734375" customWidth="1"/>
+    <col min="22" max="22" width="5.8359375" customWidth="1"/>
+    <col min="23" max="23" width="6.8671875" customWidth="1"/>
+    <col min="24" max="24" width="4.48046875" customWidth="1"/>
+    <col min="25" max="25" width="11.875" customWidth="1"/>
+    <col min="26" max="26" width="14.46484375" customWidth="1"/>
+    <col min="27" max="27" width="18.33203125" customWidth="1"/>
+    <col min="28" max="28" width="16.2890625" customWidth="1"/>
+    <col min="29" max="29" width="11.80859375" customWidth="1"/>
+    <col min="30" max="30" width="13.60546875" customWidth="1"/>
+    <col min="31" max="31" width="11.65234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -906,7 +1515,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -985,7 +1594,7 @@
       </c>
       <c r="AE2" s="1"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1064,7 +1673,7 @@
       </c>
       <c r="AE3" s="1"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1143,7 +1752,7 @@
       </c>
       <c r="AE4" s="1"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -1222,7 +1831,7 @@
       </c>
       <c r="AE5" s="1"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -1301,7 +1910,7 @@
       </c>
       <c r="AE6" s="1"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1367,7 +1976,7 @@
         <v>0</v>
       </c>
       <c r="AA7" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB7" s="1">
         <v>0</v>
@@ -1380,7 +1989,7 @@
       </c>
       <c r="AE7" s="1"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1459,7 +2068,7 @@
       </c>
       <c r="AE8" s="1"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1538,7 +2147,7 @@
       </c>
       <c r="AE9" s="1"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1617,7 +2226,7 @@
       </c>
       <c r="AE10" s="1"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -1696,7 +2305,7 @@
       </c>
       <c r="AE11" s="1"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -1775,7 +2384,7 @@
       </c>
       <c r="AE12" s="1"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1854,7 +2463,7 @@
       </c>
       <c r="AE13" s="1"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -1920,7 +2529,7 @@
         <v>0</v>
       </c>
       <c r="AA14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB14" s="1">
         <v>0</v>
@@ -1933,7 +2542,7 @@
       </c>
       <c r="AE14" s="1"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -2012,7 +2621,7 @@
       </c>
       <c r="AE15" s="1"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -2091,7 +2700,7 @@
       </c>
       <c r="AE16" s="1"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -2170,7 +2779,7 @@
       </c>
       <c r="AE17" s="1"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -2249,7 +2858,7 @@
       </c>
       <c r="AE18" s="1"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -2328,7 +2937,7 @@
       </c>
       <c r="AE19" s="1"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -2407,7 +3016,7 @@
       </c>
       <c r="AE20" s="1"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -2475,7 +3084,7 @@
         <v>0</v>
       </c>
       <c r="AA21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB21" s="1">
         <v>0</v>
@@ -2488,7 +3097,7 @@
       </c>
       <c r="AE21" s="1"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -2569,7 +3178,7 @@
       </c>
       <c r="AE22" s="1"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
@@ -2650,7 +3259,7 @@
       </c>
       <c r="AE23" s="1"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>123</v>
       </c>
@@ -2729,7 +3338,7 @@
       </c>
       <c r="AE24" s="1"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>123</v>
       </c>
@@ -2808,7 +3417,7 @@
       </c>
       <c r="AE25" s="1"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26">
       <c r="A26" s="1" t="s">
         <v>123</v>
       </c>
@@ -2887,7 +3496,7 @@
       </c>
       <c r="AE26" s="1"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27">
       <c r="A27" s="1" t="s">
         <v>123</v>
       </c>
@@ -2953,7 +3562,7 @@
         <v>0</v>
       </c>
       <c r="AA27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB27" s="1">
         <v>0</v>
@@ -2966,7 +3575,7 @@
       </c>
       <c r="AE27" s="1"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28">
       <c r="A28" s="1" t="s">
         <v>123</v>
       </c>
@@ -3032,7 +3641,7 @@
         <v>0</v>
       </c>
       <c r="AA28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB28" s="1">
         <v>0</v>
@@ -3045,7 +3654,7 @@
       </c>
       <c r="AE28" s="1"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29">
       <c r="A29" s="1" t="s">
         <v>123</v>
       </c>
@@ -3111,7 +3720,7 @@
         <v>0</v>
       </c>
       <c r="AA29" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB29" s="1">
         <v>0</v>
@@ -3124,7 +3733,7 @@
       </c>
       <c r="AE29" s="1"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30">
       <c r="A30" s="1" t="s">
         <v>123</v>
       </c>
@@ -3203,7 +3812,7 @@
       </c>
       <c r="AE30" s="1"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31">
       <c r="A31" s="1" t="s">
         <v>123</v>
       </c>
@@ -3282,7 +3891,7 @@
       </c>
       <c r="AE31" s="1"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32">
       <c r="A32" s="1" t="s">
         <v>123</v>
       </c>
@@ -3363,5 +3972,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup usePrinterDefaults="0"/>
 </worksheet>
 </file>
</xml_diff>